<commit_message>
updating presentation and readme
</commit_message>
<xml_diff>
--- a/03_Materials/finalize_stimuli/de/de_translate_final.xlsx
+++ b/03_Materials/finalize_stimuli/de/de_translate_final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erinbuchanan/GitHub/Research/2_projects/SPAML/SPAML-PSA/03_Materials/finalize_stimuli/de/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB00EC8-BA81-D74B-AF0D-C44054F668DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D4EED70-049F-524D-AC7C-3AD26E954763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8098" uniqueCount="7592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8099" uniqueCount="7595">
   <si>
     <t>de_cue</t>
   </si>
@@ -22812,6 +22812,15 @@
   </si>
   <si>
     <t>schwerfällig</t>
+  </si>
+  <si>
+    <t>Abfassung</t>
+  </si>
+  <si>
+    <t>Lesung</t>
+  </si>
+  <si>
+    <t>rasch</t>
   </si>
 </sst>
 </file>
@@ -23140,8 +23149,8 @@
   <dimension ref="A1:R1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A845" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D865" sqref="D865"/>
+      <pane ySplit="1" topLeftCell="A487" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F506" sqref="F506"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23299,7 +23308,7 @@
       </c>
       <c r="N3" s="15"/>
       <c r="P3" s="16" t="str">
-        <f t="shared" ref="P3:P66" si="3">M3</f>
+        <f t="shared" ref="P3:P64" si="3">M3</f>
         <v>abstei</v>
       </c>
       <c r="Q3" s="1" t="s">
@@ -26257,7 +26266,7 @@
       </c>
       <c r="J67" s="11"/>
       <c r="L67" s="11" t="str">
-        <f t="shared" ref="L67:L130" si="31">I67</f>
+        <f t="shared" ref="L67:L129" si="31">I67</f>
         <v>einhaft</v>
       </c>
       <c r="M67" s="15" t="s">
@@ -26265,7 +26274,7 @@
       </c>
       <c r="N67" s="15"/>
       <c r="P67" s="16" t="str">
-        <f t="shared" ref="P67:P130" si="32">M67</f>
+        <f t="shared" ref="P67:P129" si="32">M67</f>
         <v>senfahrt</v>
       </c>
       <c r="Q67" s="1" t="s">
@@ -29258,7 +29267,7 @@
       </c>
       <c r="N132" s="15"/>
       <c r="P132" s="16" t="str">
-        <f t="shared" ref="P131:P194" si="53">M132</f>
+        <f t="shared" ref="P132:P193" si="53">M132</f>
         <v>netden</v>
       </c>
       <c r="Q132" s="1" t="s">
@@ -32184,7 +32193,7 @@
       </c>
       <c r="J195" s="11"/>
       <c r="L195" s="11" t="str">
-        <f t="shared" ref="L195:L258" si="84">I195</f>
+        <f t="shared" ref="L195:L257" si="84">I195</f>
         <v>romannings</v>
       </c>
       <c r="M195" s="15" t="s">
@@ -35131,7 +35140,7 @@
       </c>
       <c r="J259" s="11"/>
       <c r="L259" s="11" t="str">
-        <f t="shared" ref="L259:L322" si="119">I259</f>
+        <f t="shared" ref="L259:L321" si="119">I259</f>
         <v>brüment</v>
       </c>
       <c r="M259" s="15" t="s">
@@ -35139,7 +35148,7 @@
       </c>
       <c r="N259" s="15"/>
       <c r="P259" s="16" t="str">
-        <f t="shared" ref="P259:P322" si="120">M259</f>
+        <f t="shared" ref="P259:P320" si="120">M259</f>
         <v>settor</v>
       </c>
       <c r="Q259" s="1" t="s">
@@ -38103,7 +38112,7 @@
       </c>
       <c r="J323" s="11"/>
       <c r="L323" s="11" t="str">
-        <f t="shared" ref="L323:L386" si="147">I323</f>
+        <f t="shared" ref="L323:L384" si="147">I323</f>
         <v>konpier</v>
       </c>
       <c r="M323" s="15" t="s">
@@ -38163,7 +38172,7 @@
       </c>
       <c r="N324" s="15"/>
       <c r="P324" s="16" t="str">
-        <f t="shared" ref="P323:P386" si="148">M324</f>
+        <f t="shared" ref="P324:P386" si="148">M324</f>
         <v>geless</v>
       </c>
       <c r="Q324" s="1" t="s">
@@ -41113,7 +41122,7 @@
       </c>
       <c r="J388" s="11"/>
       <c r="L388" s="11" t="str">
-        <f t="shared" ref="L387:L450" si="180">I388</f>
+        <f t="shared" ref="L388:L450" si="180">I388</f>
         <v>molie</v>
       </c>
       <c r="M388" s="15" t="s">
@@ -41121,7 +41130,7 @@
       </c>
       <c r="N388" s="15"/>
       <c r="P388" s="16" t="str">
-        <f t="shared" ref="P387:P450" si="181">M388</f>
+        <f t="shared" ref="P388:P450" si="181">M388</f>
         <v>holos</v>
       </c>
       <c r="Q388" s="1" t="s">
@@ -46558,13 +46567,13 @@
         <v>langsam</v>
       </c>
       <c r="E506" s="4" t="s">
-        <v>2849</v>
+        <v>7594</v>
       </c>
       <c r="F506" s="4"/>
       <c r="G506" s="4"/>
       <c r="H506" s="4" t="str">
         <f t="shared" si="201"/>
-        <v>schnell</v>
+        <v>rasch</v>
       </c>
       <c r="I506" s="11" t="s">
         <v>2850</v>
@@ -46805,7 +46814,7 @@
         <v>7181</v>
       </c>
       <c r="L511" s="11" t="str">
-        <f t="shared" ref="L511:L513" si="220">J511</f>
+        <f t="shared" ref="L511:L512" si="220">J511</f>
         <v>Milazeit</v>
       </c>
       <c r="M511" s="15" t="s">
@@ -47202,22 +47211,21 @@
     </row>
     <row r="520" spans="1:18" ht="13" x14ac:dyDescent="0.15">
       <c r="A520" s="7" t="s">
-        <v>2921</v>
+        <v>7593</v>
       </c>
       <c r="B520" s="7"/>
       <c r="C520" s="7"/>
       <c r="D520" s="7" t="str">
         <f t="shared" si="203"/>
-        <v>lesen</v>
+        <v>Lesung</v>
       </c>
       <c r="E520" s="4" t="s">
         <v>2922</v>
       </c>
       <c r="F520" s="4"/>
       <c r="G520" s="4"/>
-      <c r="H520" s="4" t="str">
-        <f t="shared" si="223"/>
-        <v>schreiben</v>
+      <c r="H520" s="4" t="s">
+        <v>7592</v>
       </c>
       <c r="I520" s="11" t="s">
         <v>2923</v>
@@ -49954,7 +49962,7 @@
       </c>
       <c r="N579" s="15"/>
       <c r="P579" s="16" t="str">
-        <f t="shared" ref="P579:P642" si="248">M579</f>
+        <f t="shared" ref="P579:P641" si="248">M579</f>
         <v>molon</v>
       </c>
       <c r="Q579" s="1" t="s">
@@ -59518,7 +59526,7 @@
         <v>7280</v>
       </c>
       <c r="L786" s="11" t="str">
-        <f t="shared" ref="L785:L786" si="332">J786</f>
+        <f t="shared" ref="L786" si="332">J786</f>
         <v>schlo</v>
       </c>
       <c r="M786" s="15" t="s">
@@ -59897,7 +59905,7 @@
         <v>7288</v>
       </c>
       <c r="L794" s="11" t="str">
-        <f t="shared" ref="L793:L794" si="338">J794</f>
+        <f t="shared" ref="L794" si="338">J794</f>
         <v>Mittenessen</v>
       </c>
       <c r="M794" s="15" t="s">

</xml_diff>